<commit_message>
update sterbedaten kw 48 destatis
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2020-12-27.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2020-12-27.xlsx
@@ -352,94 +352,94 @@
     <t xml:space="preserve">Todesfälle &amp; Sterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 47</t>
+    <t xml:space="preserve">KW 48</t>
   </si>
   <si>
     <t xml:space="preserve">0 bis 59 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">70 ( 0,1%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">83 ( 0,1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  18,6%</t>
+    <t xml:space="preserve">82 ( 0,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -1,2%</t>
   </si>
   <si>
     <t xml:space="preserve">60 bis 79 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">470 ( 2,7%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">688 ( 3,8%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  46,4%</t>
+    <t xml:space="preserve">688 ( 3,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0,0%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
   </si>
   <si>
-    <t xml:space="preserve">1126 (15,2%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1876 (17,4%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  66,6%</t>
+    <t xml:space="preserve">1985 (16,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5,8%</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">1667 ( 1,3%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2648 ( 2,1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  58,8%</t>
+    <t xml:space="preserve">2757 ( 2,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4,1%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">-104 (-6,2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-76 (-4,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -26,9%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-32 (-0,5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34 ( 0,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-206,2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1256 (12,7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1665 (16,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  32,6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1120 ( 6,3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1623 ( 9,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  44,9%</t>
+    <t xml:space="preserve">-32 (-1,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-102 (-6,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">218,8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126 ( 2,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">117 ( 1,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -7,1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1753 (17,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2510 (24,5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43,2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1846 (10,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2525 (13,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36,8%</t>
   </si>
   <si>
     <t xml:space="preserve">Vorwarnzeit</t>

</xml_diff>